<commit_message>
Changes on  Report Template
</commit_message>
<xml_diff>
--- a/OMReportTemplate.xlsx
+++ b/OMReportTemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ebcal\Source\Repos\OCMS1\OCMS\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -97,7 +97,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -121,22 +121,46 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -146,28 +170,46 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -451,30 +493,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11" style="10" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" style="10" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" style="10" customWidth="1"/>
+    <col min="4" max="4" width="8" style="10" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" style="10" customWidth="1"/>
+    <col min="6" max="6" width="4.42578125" style="10" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" style="10" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" style="11" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" style="10" customWidth="1"/>
+    <col min="10" max="10" width="8.7109375" style="10" customWidth="1"/>
+    <col min="11" max="11" width="20.85546875" style="11" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" style="10" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" style="10" customWidth="1"/>
+    <col min="14" max="14" width="20.85546875" style="11" customWidth="1"/>
+    <col min="15" max="15" width="10.7109375" style="10" customWidth="1"/>
+    <col min="16" max="16" width="8.7109375" style="10" customWidth="1"/>
+    <col min="17" max="18" width="20.85546875" style="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="18.75" x14ac:dyDescent="0.25">
@@ -483,123 +524,123 @@
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="12"/>
       <c r="I1"/>
       <c r="J1"/>
-      <c r="K1"/>
+      <c r="K1" s="12"/>
       <c r="L1"/>
       <c r="M1"/>
-      <c r="N1"/>
+      <c r="N1" s="12"/>
       <c r="O1"/>
       <c r="P1"/>
       <c r="Q1"/>
       <c r="R1"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
       <c r="H2" s="5">
         <v>1</v>
       </c>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="7"/>
       <c r="K2" s="5">
         <v>2</v>
       </c>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="7"/>
       <c r="N2" s="5">
         <v>3</v>
       </c>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="7"/>
       <c r="Q2"/>
       <c r="R2"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="M3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="N3" s="6" t="s">
+      <c r="N3" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="O3" s="6" t="s">
+      <c r="O3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="P3" s="6" t="s">
+      <c r="P3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="Q3" s="6" t="s">
+      <c r="Q3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="R3" s="6" t="s">
+      <c r="R3" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="7"/>
-      <c r="R4" s="7"/>
+      <c r="A4" s="8"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="8"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>